<commit_message>
update to excel 2
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pc2\test123\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECBFE5D-5733-42E6-AE89-377D528E8DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BE00EE-FB52-484C-B68B-B095EA7D5B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ورقة1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>jana</t>
+  </si>
+  <si>
+    <t>mark</t>
   </si>
 </sst>
 </file>
@@ -357,44 +360,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
+      <c r="C3">
+        <v>80</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>3</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>